<commit_message>
Added periority to test case, todo: add comments
</commit_message>
<xml_diff>
--- a/Testcase.xlsx
+++ b/Testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planittesting-my.sharepoint.com/personal/bliu_planittesting_com/Documents/Desktop/SDET bootcamp/saucedemoJavaAutomationTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="13_ncr:1_{65865187-4587-4C1C-BA1D-94FF3B1412F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F27049-5844-4796-9280-C1F058C5B354}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{65865187-4587-4C1C-BA1D-94FF3B1412F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFD35BFC-856C-44E7-A155-EAE5076334AA}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
-  <si>
-    <t>Test Case Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
   <si>
     <t>TC10</t>
   </si>
@@ -234,6 +231,21 @@
   <si>
     <t>On Chech out step one page, with url 
 containing "checkout-step-one"</t>
+  </si>
+  <si>
+    <t>Test Case Num</t>
+  </si>
+  <si>
+    <t>Periority</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -283,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -306,12 +318,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -326,6 +351,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -609,397 +637,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:F25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="D20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="D21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="E23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="G24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>15</v>
+      <c r="G25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>